<commit_message>
Last update transloc CMR
</commit_message>
<xml_diff>
--- a/data/NewlyCreatedData/Checks/idade_checks_v2.xlsx
+++ b/data/NewlyCreatedData/Checks/idade_checks_v2.xlsx
@@ -344,13 +344,13 @@
     <t>obs20597</t>
   </si>
   <si>
-    <t>obs20791</t>
-  </si>
-  <si>
-    <t>obs20973</t>
-  </si>
-  <si>
-    <t>obs21166</t>
+    <t>obs20790</t>
+  </si>
+  <si>
+    <t>obs20972</t>
+  </si>
+  <si>
+    <t>obs21165</t>
   </si>
   <si>
     <t>obs7222</t>
@@ -662,16 +662,16 @@
     <t>obs20190</t>
   </si>
   <si>
-    <t>obs20600</t>
-  </si>
-  <si>
-    <t>obs20793</t>
-  </si>
-  <si>
-    <t>obs20975</t>
-  </si>
-  <si>
-    <t>obs21168</t>
+    <t>obs20599</t>
+  </si>
+  <si>
+    <t>obs20792</t>
+  </si>
+  <si>
+    <t>obs20974</t>
+  </si>
+  <si>
+    <t>obs21167</t>
   </si>
   <si>
     <t>obs1219</t>
@@ -719,6 +719,48 @@
     <t>obs11541</t>
   </si>
   <si>
+    <t>obs22146</t>
+  </si>
+  <si>
+    <t>obs22352</t>
+  </si>
+  <si>
+    <t>obs22574</t>
+  </si>
+  <si>
+    <t>obs22810</t>
+  </si>
+  <si>
+    <t>obs23057</t>
+  </si>
+  <si>
+    <t>obs23323</t>
+  </si>
+  <si>
+    <t>obs23605</t>
+  </si>
+  <si>
+    <t>obs23914</t>
+  </si>
+  <si>
+    <t>obs24238</t>
+  </si>
+  <si>
+    <t>obs24565</t>
+  </si>
+  <si>
+    <t>obs24913</t>
+  </si>
+  <si>
+    <t>obs25275</t>
+  </si>
+  <si>
+    <t>obs25652</t>
+  </si>
+  <si>
+    <t>obs26061</t>
+  </si>
+  <si>
     <t>obs22147</t>
   </si>
   <si>
@@ -731,78 +773,78 @@
     <t>obs22811</t>
   </si>
   <si>
+    <t>obs23105</t>
+  </si>
+  <si>
+    <t>obs23324</t>
+  </si>
+  <si>
+    <t>obs23606</t>
+  </si>
+  <si>
+    <t>obs23915</t>
+  </si>
+  <si>
+    <t>obs24239</t>
+  </si>
+  <si>
+    <t>obs24566</t>
+  </si>
+  <si>
+    <t>obs24914</t>
+  </si>
+  <si>
+    <t>obs25276</t>
+  </si>
+  <si>
+    <t>obs25653</t>
+  </si>
+  <si>
+    <t>obs26062</t>
+  </si>
+  <si>
+    <t>obs22354</t>
+  </si>
+  <si>
+    <t>obs22576</t>
+  </si>
+  <si>
+    <t>obs22812</t>
+  </si>
+  <si>
     <t>obs23058</t>
   </si>
   <si>
-    <t>obs23324</t>
-  </si>
-  <si>
-    <t>obs23606</t>
-  </si>
-  <si>
-    <t>obs23915</t>
-  </si>
-  <si>
-    <t>obs24239</t>
-  </si>
-  <si>
-    <t>obs24566</t>
-  </si>
-  <si>
-    <t>obs24914</t>
-  </si>
-  <si>
-    <t>obs25276</t>
-  </si>
-  <si>
-    <t>obs25653</t>
-  </si>
-  <si>
-    <t>obs26062</t>
+    <t>obs23325</t>
+  </si>
+  <si>
+    <t>obs23607</t>
+  </si>
+  <si>
+    <t>obs23916</t>
+  </si>
+  <si>
+    <t>obs24240</t>
+  </si>
+  <si>
+    <t>obs24567</t>
+  </si>
+  <si>
+    <t>obs24915</t>
+  </si>
+  <si>
+    <t>obs25277</t>
+  </si>
+  <si>
+    <t>obs25654</t>
+  </si>
+  <si>
+    <t>obs26063</t>
   </si>
   <si>
     <t>obs22148</t>
   </si>
   <si>
-    <t>obs22354</t>
-  </si>
-  <si>
-    <t>obs22576</t>
-  </si>
-  <si>
-    <t>obs22812</t>
-  </si>
-  <si>
-    <t>obs23106</t>
-  </si>
-  <si>
-    <t>obs23325</t>
-  </si>
-  <si>
-    <t>obs23607</t>
-  </si>
-  <si>
-    <t>obs23916</t>
-  </si>
-  <si>
-    <t>obs24240</t>
-  </si>
-  <si>
-    <t>obs24567</t>
-  </si>
-  <si>
-    <t>obs24915</t>
-  </si>
-  <si>
-    <t>obs25277</t>
-  </si>
-  <si>
-    <t>obs25654</t>
-  </si>
-  <si>
-    <t>obs26063</t>
-  </si>
-  <si>
     <t>obs22355</t>
   </si>
   <si>
@@ -842,64 +884,55 @@
     <t>obs26064</t>
   </si>
   <si>
-    <t>obs22149</t>
-  </si>
-  <si>
-    <t>obs22356</t>
-  </si>
-  <si>
-    <t>obs22578</t>
-  </si>
-  <si>
-    <t>obs22814</t>
-  </si>
-  <si>
-    <t>obs23060</t>
-  </si>
-  <si>
-    <t>obs23327</t>
-  </si>
-  <si>
-    <t>obs23609</t>
-  </si>
-  <si>
-    <t>obs23918</t>
-  </si>
-  <si>
-    <t>obs24242</t>
-  </si>
-  <si>
-    <t>obs24569</t>
-  </si>
-  <si>
-    <t>obs24917</t>
-  </si>
-  <si>
-    <t>obs25279</t>
-  </si>
-  <si>
-    <t>obs25656</t>
-  </si>
-  <si>
-    <t>obs26065</t>
-  </si>
-  <si>
-    <t>obs22154</t>
-  </si>
-  <si>
-    <t>obs22361</t>
-  </si>
-  <si>
-    <t>obs22583</t>
-  </si>
-  <si>
-    <t>obs22817</t>
-  </si>
-  <si>
-    <t>obs23063</t>
-  </si>
-  <si>
-    <t>obs23330</t>
+    <t>obs22153</t>
+  </si>
+  <si>
+    <t>obs22360</t>
+  </si>
+  <si>
+    <t>obs22582</t>
+  </si>
+  <si>
+    <t>obs22816</t>
+  </si>
+  <si>
+    <t>obs23062</t>
+  </si>
+  <si>
+    <t>obs23329</t>
+  </si>
+  <si>
+    <t>obs23611</t>
+  </si>
+  <si>
+    <t>obs23919</t>
+  </si>
+  <si>
+    <t>obs24297</t>
+  </si>
+  <si>
+    <t>obs24570</t>
+  </si>
+  <si>
+    <t>obs24918</t>
+  </si>
+  <si>
+    <t>obs25280</t>
+  </si>
+  <si>
+    <t>obs25657</t>
+  </si>
+  <si>
+    <t>obs26066</t>
+  </si>
+  <si>
+    <t>obs22853</t>
+  </si>
+  <si>
+    <t>obs23107</t>
+  </si>
+  <si>
+    <t>obs23371</t>
   </si>
   <si>
     <t>obs23612</t>
@@ -908,7 +941,7 @@
     <t>obs23920</t>
   </si>
   <si>
-    <t>obs24298</t>
+    <t>obs24299</t>
   </si>
   <si>
     <t>obs24571</t>
@@ -923,73 +956,64 @@
     <t>obs25658</t>
   </si>
   <si>
+    <t>obs26070</t>
+  </si>
+  <si>
+    <t>obs22855</t>
+  </si>
+  <si>
+    <t>obs23109</t>
+  </si>
+  <si>
+    <t>obs23373</t>
+  </si>
+  <si>
+    <t>obs23613</t>
+  </si>
+  <si>
+    <t>obs23921</t>
+  </si>
+  <si>
+    <t>obs24301</t>
+  </si>
+  <si>
+    <t>obs24572</t>
+  </si>
+  <si>
+    <t>obs24920</t>
+  </si>
+  <si>
+    <t>obs25282</t>
+  </si>
+  <si>
+    <t>obs25659</t>
+  </si>
+  <si>
     <t>obs26067</t>
   </si>
   <si>
-    <t>obs22854</t>
-  </si>
-  <si>
-    <t>obs23108</t>
-  </si>
-  <si>
-    <t>obs23372</t>
-  </si>
-  <si>
-    <t>obs23613</t>
-  </si>
-  <si>
-    <t>obs23921</t>
-  </si>
-  <si>
-    <t>obs24300</t>
-  </si>
-  <si>
-    <t>obs24572</t>
-  </si>
-  <si>
-    <t>obs24920</t>
-  </si>
-  <si>
-    <t>obs25282</t>
-  </si>
-  <si>
-    <t>obs25659</t>
-  </si>
-  <si>
-    <t>obs26071</t>
-  </si>
-  <si>
-    <t>obs22856</t>
-  </si>
-  <si>
-    <t>obs23110</t>
-  </si>
-  <si>
-    <t>obs23374</t>
-  </si>
-  <si>
-    <t>obs23614</t>
-  </si>
-  <si>
-    <t>obs23922</t>
+    <t>obs23661</t>
+  </si>
+  <si>
+    <t>obs23979</t>
   </si>
   <si>
     <t>obs24302</t>
   </si>
   <si>
-    <t>obs24573</t>
-  </si>
-  <si>
-    <t>obs24921</t>
-  </si>
-  <si>
-    <t>obs25283</t>
-  </si>
-  <si>
-    <t>obs25660</t>
-  </si>
-  <si>
-    <t>obs26068</t>
+    <t>obs24629</t>
+  </si>
+  <si>
+    <t>obs24981</t>
+  </si>
+  <si>
+    <t>obs25343</t>
+  </si>
+  <si>
+    <t>obs25726</t>
+  </si>
+  <si>
+    <t>obs26160</t>
   </si>
   <si>
     <t>obs23662</t>
@@ -1040,40 +1064,16 @@
     <t>obs26162</t>
   </si>
   <si>
-    <t>obs23664</t>
-  </si>
-  <si>
-    <t>obs23982</t>
-  </si>
-  <si>
-    <t>obs24305</t>
-  </si>
-  <si>
-    <t>obs24632</t>
-  </si>
-  <si>
-    <t>obs24984</t>
-  </si>
-  <si>
-    <t>obs25346</t>
-  </si>
-  <si>
-    <t>obs25729</t>
-  </si>
-  <si>
-    <t>obs26163</t>
+    <t>obs25680</t>
+  </si>
+  <si>
+    <t>obs26100</t>
   </si>
   <si>
     <t>obs25681</t>
   </si>
   <si>
     <t>obs26101</t>
-  </si>
-  <si>
-    <t>obs25682</t>
-  </si>
-  <si>
-    <t>obs26102</t>
   </si>
   <si>
     <t>obs536</t>

</xml_diff>